<commit_message>
Cannibas and Zillow Update
</commit_message>
<xml_diff>
--- a/images/Zillow/Raw Data/_ZHVI Data/City_ZHVI_ByType.xlsx
+++ b/images/Zillow/Raw Data/_ZHVI Data/City_ZHVI_ByType.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1960" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1967" uniqueCount="281">
   <si>
     <t>Date</t>
   </si>
@@ -858,6 +858,9 @@
   </si>
   <si>
     <t>2019-06-01</t>
+  </si>
+  <si>
+    <t>2019-07-01</t>
   </si>
 </sst>
 </file>
@@ -2308,6 +2311,11 @@
         <v>279</v>
       </c>
     </row>
+    <row r="281">
+      <c r="A281" t="s">
+        <v>280</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -3721,6 +3729,11 @@
         <v>279</v>
       </c>
     </row>
+    <row r="281">
+      <c r="A281" t="s">
+        <v>280</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -5134,6 +5147,11 @@
         <v>279</v>
       </c>
     </row>
+    <row r="281">
+      <c r="A281" t="s">
+        <v>280</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -6547,6 +6565,11 @@
         <v>279</v>
       </c>
     </row>
+    <row r="281">
+      <c r="A281" t="s">
+        <v>280</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -7960,6 +7983,11 @@
         <v>279</v>
       </c>
     </row>
+    <row r="281">
+      <c r="A281" t="s">
+        <v>280</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -9373,6 +9401,11 @@
         <v>279</v>
       </c>
     </row>
+    <row r="281">
+      <c r="A281" t="s">
+        <v>280</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -10786,6 +10819,11 @@
         <v>279</v>
       </c>
     </row>
+    <row r="281">
+      <c r="A281" t="s">
+        <v>280</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>